<commit_message>
finished 3.3V PLC modul with atmega & sig 60
</commit_message>
<xml_diff>
--- a/BuckBoost/Results.xlsx
+++ b/BuckBoost/Results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -53,6 +54,58 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Supply</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Supply</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Supply</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>U</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -69,22 +122,7 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Supply</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>U</t>
-    </r>
-    <r>
-      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -101,38 +139,7 @@
     </r>
     <r>
       <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Supply</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>P</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Supply</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -149,6 +156,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -165,6 +173,7 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -179,11 +188,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +201,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,15 +218,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -216,16 +246,175 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -271,6 +460,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Voltagelevels</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -302,7 +516,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14088574074074073"/>
+          <c:y val="0.13945305555555557"/>
+          <c:w val="0.80916055555555555"/>
+          <c:h val="0.67460388888888889"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -332,6 +556,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.385</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$B$2:$B$21</c:f>
@@ -434,6 +727,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.385</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$E$2:$E$21</c:f>
@@ -536,6 +898,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$G$2:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.385</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Tabelle1!$F$2:$F$21</c:f>
@@ -661,7 +1092,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>I</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="-25000"/>
+                  <a:t>con</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> [A]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -727,6 +1221,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>U [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -781,7 +1330,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79012037037037042"/>
+          <c:y val="0.1752761111111111"/>
+          <c:w val="0.14167592592592593"/>
+          <c:h val="0.178595"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -817,14 +1376,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="accent4">
+        <a:lumMod val="20000"/>
+        <a:lumOff val="80000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -863,6 +1422,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Powerflow</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -894,7 +1478,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14088574074074073"/>
+          <c:y val="0.13945305555555557"/>
+          <c:w val="0.81415833333333332"/>
+          <c:h val="0.67460388888888889"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -926,69 +1520,69 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$21</c:f>
+              <c:f>Tabelle1!$G$2:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2</c:v>
+                  <c:v>1.19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3</c:v>
+                  <c:v>1.29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4</c:v>
+                  <c:v>1.385</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5</c:v>
+                  <c:v>1.49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.7</c:v>
+                  <c:v>1.69</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8</c:v>
+                  <c:v>1.79</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>1.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1097,69 +1691,69 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$21</c:f>
+              <c:f>Tabelle1!$G$2:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2</c:v>
+                  <c:v>1.19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3</c:v>
+                  <c:v>1.29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4</c:v>
+                  <c:v>1.385</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5</c:v>
+                  <c:v>1.49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.7</c:v>
+                  <c:v>1.69</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8</c:v>
+                  <c:v>1.79</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>1.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,69 +1862,69 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$2:$A$21</c:f>
+              <c:f>Tabelle1!$G$2:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.3</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.6</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.9</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2</c:v>
+                  <c:v>1.19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.3</c:v>
+                  <c:v>1.29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.4</c:v>
+                  <c:v>1.385</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5</c:v>
+                  <c:v>1.49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.7</c:v>
+                  <c:v>1.69</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8</c:v>
+                  <c:v>1.79</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>1.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,7 +2054,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>I</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="-25000"/>
+                  <a:t>con</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> [A]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1526,6 +2184,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>P [W]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1580,7 +2293,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79276629629629625"/>
+          <c:y val="0.161165"/>
+          <c:w val="0.13902999999999999"/>
+          <c:h val="0.178595"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1616,14 +2339,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="accent4">
+        <a:lumMod val="20000"/>
+        <a:lumOff val="80000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -2833,16 +3556,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>73620</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>110040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2869,16 +3592,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>149820</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>87180</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3202,11 +3925,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3215,734 +3938,734 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="A2" s="7">
         <v>0.1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>12</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="8">
         <f>B2*C2</f>
         <v>3.3600000000000003</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="8">
         <v>14.45</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="8">
         <v>12.1</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="8">
         <v>0.1</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="8">
         <f>F2*G2</f>
         <v>1.21</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="8">
         <f>D2-H2</f>
         <v>2.1500000000000004</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="A3" s="7">
         <v>0.2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="8">
         <v>12</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="8">
         <v>0.38</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <f t="shared" ref="D3:D21" si="0">B3*C3</f>
         <v>4.5600000000000005</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>14.45</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="8">
         <v>12.1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="8">
         <v>0.19</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="8">
         <f t="shared" ref="H3:H21" si="1">F3*G3</f>
         <v>2.2989999999999999</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="8">
         <f t="shared" ref="I3:I21" si="2">D3-H3</f>
         <v>2.2610000000000006</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4" s="7">
         <v>0.3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="8">
         <v>12</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="8">
         <v>0.51</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <f t="shared" si="0"/>
         <v>6.12</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>14.46</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="8">
         <v>12.1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="8">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="8">
         <f t="shared" si="1"/>
         <v>3.5089999999999995</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="8">
         <f t="shared" si="2"/>
         <v>2.6110000000000007</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="7">
         <v>0.4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="8">
         <v>12</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
         <v>0.63</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="8">
         <f t="shared" si="0"/>
         <v>7.5600000000000005</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="8">
         <v>14.48</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="8">
         <v>12.1</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="8">
         <v>0.4</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="8">
         <f t="shared" si="1"/>
         <v>4.84</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="8">
         <f t="shared" si="2"/>
         <v>2.7200000000000006</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="A6" s="7">
         <v>0.5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="8">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="8">
         <v>0.73499999999999999</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="8">
         <f t="shared" si="0"/>
         <v>8.82</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="8">
         <v>14.48</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="8">
         <v>12.1</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="8">
         <v>0.48</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="8">
         <f t="shared" si="1"/>
         <v>5.8079999999999998</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="8">
         <f t="shared" si="2"/>
         <v>3.0120000000000005</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="A7" s="7">
         <v>0.6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="8">
         <v>12</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <v>0.86</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="8">
         <f t="shared" si="0"/>
         <v>10.32</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="8">
         <v>14.47</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="8">
         <v>12.1</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="8">
         <v>0.59</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="8">
         <f t="shared" si="1"/>
         <v>7.1389999999999993</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="8">
         <f t="shared" si="2"/>
         <v>3.1810000000000009</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8" s="7">
         <v>0.7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="8">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="8">
         <v>0.99</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="8">
         <f t="shared" si="0"/>
         <v>11.879999999999999</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
         <v>14.47</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="8">
         <v>12.1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="8">
         <v>0.69</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="8">
         <f t="shared" si="1"/>
         <v>8.3489999999999984</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="8">
         <f t="shared" si="2"/>
         <v>3.5310000000000006</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9" s="7">
         <v>0.8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="8">
         <v>12</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="8">
         <v>1.0900000000000001</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="8">
         <f t="shared" si="0"/>
         <v>13.080000000000002</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
         <v>14.46</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="8">
         <v>12.1</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="8">
         <v>0.78</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="8">
         <f t="shared" si="1"/>
         <v>9.4380000000000006</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="8">
         <f t="shared" si="2"/>
         <v>3.6420000000000012</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="A10" s="7">
         <v>0.9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="8">
         <v>12</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
         <v>1.22</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <f t="shared" si="0"/>
         <v>14.64</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>14.46</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="8">
         <v>12.1</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="8">
         <v>0.89</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="8">
         <f t="shared" si="1"/>
         <v>10.769</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="8">
         <f t="shared" si="2"/>
         <v>3.8710000000000004</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="A11" s="7">
         <v>1</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="8">
         <v>10.5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="8">
         <v>1.35</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="8">
         <f t="shared" si="0"/>
         <v>14.175000000000001</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="8">
         <v>14.45</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="8">
         <v>12</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="8">
         <v>0.99</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="8">
         <f t="shared" si="1"/>
         <v>11.879999999999999</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="8">
         <f t="shared" si="2"/>
         <v>2.2950000000000017</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="A12" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="8">
         <v>10.3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="8">
         <v>1.46</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="8">
         <f t="shared" si="0"/>
         <v>15.038</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
         <v>14.45</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="8">
         <v>10.6</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="8">
         <v>1.08</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="8">
         <f t="shared" si="1"/>
         <v>11.448</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="8">
         <f t="shared" si="2"/>
         <v>3.59</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="A13" s="7">
         <v>1.2</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="8">
         <v>10.3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="8">
         <v>1.58</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="8">
         <f t="shared" si="0"/>
         <v>16.274000000000001</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="8">
         <v>10.63</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="8">
         <v>9.4</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="8">
         <v>1.19</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="8">
         <f t="shared" si="1"/>
         <v>11.186</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="8">
         <f t="shared" si="2"/>
         <v>5.088000000000001</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+      <c r="A14" s="7">
         <v>1.3</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="8">
         <v>10.4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="8">
         <v>1.58</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="8">
         <f t="shared" si="0"/>
         <v>16.432000000000002</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="8">
         <v>10.220000000000001</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="8">
         <v>8.9</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="8">
         <v>1.29</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="8">
         <f t="shared" si="1"/>
         <v>11.481000000000002</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="8">
         <f t="shared" si="2"/>
         <v>4.9510000000000005</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="A15" s="7">
         <v>1.4</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="8">
         <v>10.5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="8">
         <v>1.58</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="8">
         <f t="shared" si="0"/>
         <v>16.59</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="8">
         <v>10.02</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="8">
         <v>8.6</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="8">
         <v>1.385</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="8">
         <f t="shared" si="1"/>
         <v>11.911</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="8">
         <f t="shared" si="2"/>
         <v>4.6790000000000003</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+      <c r="A16" s="7">
         <v>1.5</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="8">
         <v>7.6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="8">
         <v>1.58</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="8">
         <f t="shared" si="0"/>
         <v>12.007999999999999</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
         <v>6.78</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="8">
         <v>5.2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="8">
         <v>1.49</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="8">
         <f t="shared" si="1"/>
         <v>7.7480000000000002</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="8">
         <f t="shared" si="2"/>
         <v>4.2599999999999989</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+      <c r="A17" s="7">
         <v>1.6</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="8">
         <v>6</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="8">
         <v>1.58</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="8">
         <f t="shared" si="0"/>
         <v>9.48</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="8">
         <v>5.35</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="8">
         <v>3.3</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="8">
         <v>1.6</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="8">
         <f t="shared" si="1"/>
         <v>5.28</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="8">
         <f t="shared" si="2"/>
         <v>4.2</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+      <c r="A18" s="7">
         <v>1.7</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="8">
         <v>6.1</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="8">
         <v>1.58</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="8">
         <f t="shared" si="0"/>
         <v>9.6379999999999999</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="8">
         <v>5.47</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="8">
         <v>3.2</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="8">
         <v>1.69</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="8">
         <f t="shared" si="1"/>
         <v>5.4080000000000004</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="8">
         <f t="shared" si="2"/>
         <v>4.2299999999999995</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+      <c r="A19" s="7">
         <v>1.8</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="8">
         <v>6.1</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="8">
         <v>1.58</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="8">
         <f t="shared" si="0"/>
         <v>9.6379999999999999</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="8">
         <v>5.49</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="8">
         <v>3</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="8">
         <v>1.79</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="8">
         <f t="shared" si="1"/>
         <v>5.37</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="8">
         <f t="shared" si="2"/>
         <v>4.2679999999999998</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+      <c r="A20" s="7">
         <v>1.9</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="8">
         <v>6.1</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="8">
         <v>1.58</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="8">
         <f t="shared" si="0"/>
         <v>9.6379999999999999</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="8">
         <v>5.5</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="8">
         <v>2.8</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="8">
         <v>1.9</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="8">
         <f t="shared" si="1"/>
         <v>5.3199999999999994</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="8">
         <f t="shared" si="2"/>
         <v>4.3180000000000005</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9">
         <v>2</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="10">
         <v>6.2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="10">
         <v>1.58</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="10">
         <f t="shared" si="0"/>
         <v>9.7960000000000012</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="10">
         <v>5.51</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="10">
         <v>2.6</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="10">
         <v>1.99</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="10">
         <f t="shared" si="1"/>
         <v>5.1740000000000004</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I21" s="10">
         <f t="shared" si="2"/>
         <v>4.6220000000000008</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="6" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>